<commit_message>
Updae RMR lmer results
</commit_message>
<xml_diff>
--- a/results/RMR results/lmer_ind_effects_m_basin_season.xlsx
+++ b/results/RMR results/lmer_ind_effects_m_basin_season.xlsx
@@ -53,13 +53,19 @@
     <t xml:space="preserve">fish_basinNorth</t>
   </si>
   <si>
+    <t xml:space="preserve">seasonSpring</t>
+  </si>
+  <si>
     <t xml:space="preserve">seasonSummer</t>
   </si>
   <si>
     <t xml:space="preserve">seasonFall</t>
   </si>
   <si>
-    <t xml:space="preserve">seasonWinter</t>
+    <t xml:space="preserve">fish_basinWest:seasonSpring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fish_basinNorth:seasonSpring</t>
   </si>
   <si>
     <t xml:space="preserve">fish_basinWest:seasonSummer</t>
@@ -72,12 +78,6 @@
   </si>
   <si>
     <t xml:space="preserve">fish_basinNorth:seasonFall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fish_basinWest:seasonWinter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fish_basinNorth:seasonWinter</t>
   </si>
   <si>
     <t xml:space="preserve">ran_pars</t>
@@ -462,16 +462,16 @@
         <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>69.1047171234802</v>
+        <v>63.9490421663899</v>
       </c>
       <c r="F2" t="n">
-        <v>5.84137492358458</v>
+        <v>5.84634808873611</v>
       </c>
       <c r="G2" t="n">
-        <v>11.830214295006</v>
+        <v>10.9382885171681</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0000000000000000000000000000000272445346128118</v>
+        <v>0.000000000000000000000000000756138161659184</v>
       </c>
     </row>
     <row r="3">
@@ -486,16 +486,16 @@
         <v>11</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.665164136720086</v>
+        <v>-6.92482794038639</v>
       </c>
       <c r="F3" t="n">
-        <v>9.17871912324021</v>
+        <v>9.19983626300987</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.0724680783657398</v>
+        <v>-0.752712085564969</v>
       </c>
       <c r="H3" t="n">
-        <v>0.942229408429252</v>
+        <v>0.451622945903206</v>
       </c>
     </row>
     <row r="4">
@@ -510,16 +510,16 @@
         <v>12</v>
       </c>
       <c r="E4" t="n">
-        <v>6.9669700925186</v>
+        <v>1.96775395662565</v>
       </c>
       <c r="F4" t="n">
-        <v>9.74410589714862</v>
+        <v>9.78924461576805</v>
       </c>
       <c r="G4" t="n">
-        <v>0.714993265267912</v>
+        <v>0.201011828170694</v>
       </c>
       <c r="H4" t="n">
-        <v>0.474613204783851</v>
+        <v>0.840689325293592</v>
       </c>
     </row>
     <row r="5">
@@ -534,16 +534,16 @@
         <v>13</v>
       </c>
       <c r="E5" t="n">
-        <v>13.8409062158906</v>
+        <v>5.15522888053912</v>
       </c>
       <c r="F5" t="n">
-        <v>0.96718660285748</v>
+        <v>0.939241157249013</v>
       </c>
       <c r="G5" t="n">
-        <v>14.3104817364081</v>
+        <v>5.48871697194202</v>
       </c>
       <c r="H5" t="n">
-        <v>0.000000000000000000000000000000000000000000000188205087398104</v>
+        <v>0.0000000404863738268761</v>
       </c>
     </row>
     <row r="6">
@@ -558,16 +558,16 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>12.7193465503516</v>
+        <v>18.9960979832281</v>
       </c>
       <c r="F6" t="n">
-        <v>0.958838122696969</v>
+        <v>0.984585974459425</v>
       </c>
       <c r="G6" t="n">
-        <v>13.2653742579355</v>
+        <v>19.2934883047239</v>
       </c>
       <c r="H6" t="n">
-        <v>0.000000000000000000000000000000000000000367581119513297</v>
+        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000609208018769435</v>
       </c>
     </row>
     <row r="7">
@@ -582,16 +582,16 @@
         <v>15</v>
       </c>
       <c r="E7" t="n">
-        <v>-5.15523574352672</v>
+        <v>17.8745995915453</v>
       </c>
       <c r="F7" t="n">
-        <v>0.939240764317583</v>
+        <v>0.970139778635657</v>
       </c>
       <c r="G7" t="n">
-        <v>-5.48872657509954</v>
+        <v>18.4247672193</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0000000404841731217857</v>
+        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000831475795147886</v>
       </c>
     </row>
     <row r="8">
@@ -606,16 +606,16 @@
         <v>16</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.573935833122038</v>
+        <v>6.25981986905563</v>
       </c>
       <c r="F8" t="n">
-        <v>2.09301349717984</v>
+        <v>2.26548333187795</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.274215065452453</v>
+        <v>2.76312775334639</v>
       </c>
       <c r="H8" t="n">
-        <v>0.783919351147365</v>
+        <v>0.00572503536149729</v>
       </c>
     </row>
     <row r="9">
@@ -630,16 +630,16 @@
         <v>17</v>
       </c>
       <c r="E9" t="n">
-        <v>-1.28290884535939</v>
+        <v>5.00009918075326</v>
       </c>
       <c r="F9" t="n">
-        <v>1.99524645469277</v>
+        <v>2.22682472613375</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.642982646250048</v>
+        <v>2.24539413545786</v>
       </c>
       <c r="H9" t="n">
-        <v>0.520235360353276</v>
+        <v>0.024742841569497</v>
       </c>
     </row>
     <row r="10">
@@ -654,16 +654,16 @@
         <v>18</v>
       </c>
       <c r="E10" t="n">
-        <v>6.2095144008836</v>
+        <v>5.68592769756434</v>
       </c>
       <c r="F10" t="n">
-        <v>2.09220158689257</v>
+        <v>2.1782608863092</v>
       </c>
       <c r="G10" t="n">
-        <v>2.96793312833026</v>
+        <v>2.6103061085573</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0029980954899455</v>
+        <v>0.00904612360291998</v>
       </c>
     </row>
     <row r="11">
@@ -678,16 +678,16 @@
         <v>19</v>
       </c>
       <c r="E11" t="n">
-        <v>-11.7029797001608</v>
+        <v>3.7172719328726</v>
       </c>
       <c r="F11" t="n">
-        <v>2.03208455421844</v>
+        <v>2.09387817856051</v>
       </c>
       <c r="G11" t="n">
-        <v>-5.75910075979186</v>
+        <v>1.77530477700863</v>
       </c>
       <c r="H11" t="n">
-        <v>0.00000000845632156345194</v>
+        <v>0.0758475770777054</v>
       </c>
     </row>
     <row r="12">
@@ -702,16 +702,16 @@
         <v>20</v>
       </c>
       <c r="E12" t="n">
-        <v>-6.2597839968006</v>
+        <v>12.4692733429239</v>
       </c>
       <c r="F12" t="n">
-        <v>2.26548238410292</v>
+        <v>2.17351279653477</v>
       </c>
       <c r="G12" t="n">
-        <v>-2.76311307504575</v>
+        <v>5.73692198306982</v>
       </c>
       <c r="H12" t="n">
-        <v>0.00572529283504079</v>
+        <v>0.00000000964126405643401</v>
       </c>
     </row>
     <row r="13">
@@ -726,16 +726,16 @@
         <v>21</v>
       </c>
       <c r="E13" t="n">
-        <v>-5.00009818862286</v>
+        <v>-6.70289405815238</v>
       </c>
       <c r="F13" t="n">
-        <v>2.22682379938975</v>
+        <v>2.10879038006366</v>
       </c>
       <c r="G13" t="n">
-        <v>-2.24539462439422</v>
+        <v>-3.17854923918519</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0247428102091887</v>
+        <v>0.00148014075630594</v>
       </c>
     </row>
     <row r="14">
@@ -752,7 +752,7 @@
         <v>24</v>
       </c>
       <c r="E14" t="n">
-        <v>15.2274540136856</v>
+        <v>15.2273995412183</v>
       </c>
       <c r="F14"/>
       <c r="G14"/>
@@ -772,7 +772,7 @@
         <v>26</v>
       </c>
       <c r="E15" t="n">
-        <v>14.2526957381869</v>
+        <v>14.2527016998416</v>
       </c>
       <c r="F15"/>
       <c r="G15"/>

</xml_diff>